<commit_message>
add the widgets into the main project
</commit_message>
<xml_diff>
--- a/ImportantLinks.xlsx
+++ b/ImportantLinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mok_PT1d1\MoK_PT1d2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A49063-2CCB-41E8-AFBC-F6FF0CA9DBA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6047CE8B-294F-4B08-B410-FA9238BC0F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>https://codepen.io/RajRajeshDn/details/ExxrgOp</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>icons - material angular</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/35655361/angular2-how-to-load-data-before-rendering-the-component</t>
+  </si>
+  <si>
+    <t>Getting data syncronously / Getting data after page loads so  page doesn't show data</t>
   </si>
 </sst>
 </file>
@@ -371,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,11 +413,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{86DD1B58-E270-45EF-83AF-AF3DC76222FC}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{743B7637-BB61-4BF2-9F66-3DFD93077453}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{E6F51CC8-9AE2-4705-8CF3-9E264664B7B3}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{47AA9869-B134-42A4-9997-8DE61A9ABE50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>